<commit_message>
Added a CC license to the sheet
</commit_message>
<xml_diff>
--- a/Courses Schedule.xlsx
+++ b/Courses Schedule.xlsx
@@ -7,10 +7,10 @@
     <workbookView xWindow="14385" yWindow="45" windowWidth="6105" windowHeight="8250"/>
   </bookViews>
   <sheets>
-    <sheet name="Coursera" sheetId="1" r:id="rId1"/>
+    <sheet name="Coursera courses" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Coursera!$A$1:$K$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Coursera courses'!$A$2:$K$12</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -22,7 +22,7 @@
     <author>Ahmad</author>
   </authors>
   <commentList>
-    <comment ref="E1" authorId="0">
+    <comment ref="E2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
   <si>
     <t>Verified Certificate</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>Specialization: Z</t>
+  </si>
+  <si>
+    <t>This work is licensed under a Creative Commons Attribution 4.0 International License.</t>
   </si>
 </sst>
 </file>
@@ -136,7 +139,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,6 +166,13 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -206,7 +216,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -274,6 +284,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -333,7 +350,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Coursera!$B$2:$B$11</c:f>
+              <c:f>'Coursera courses'!$B$3:$B$12</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -371,7 +388,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Coursera!$C$2:$C$11</c:f>
+              <c:f>'Coursera courses'!$C$3:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="10"/>
@@ -423,7 +440,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Coursera!$B$2:$B$11</c:f>
+              <c:f>'Coursera courses'!$B$3:$B$12</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -461,7 +478,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Coursera!$I$2:$I$11</c:f>
+              <c:f>'Coursera courses'!$I$3:$I$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -481,10 +498,10 @@
                   <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -516,7 +533,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Coursera!$B$2:$B$11</c:f>
+              <c:f>'Coursera courses'!$B$3:$B$12</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -554,7 +571,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Coursera!$J$2:$J$11</c:f>
+              <c:f>'Coursera courses'!$J$3:$J$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -574,10 +591,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>16</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>28</c:v>
@@ -602,11 +619,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="110289280"/>
-        <c:axId val="110290816"/>
+        <c:axId val="76992896"/>
+        <c:axId val="76994432"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="110289280"/>
+        <c:axId val="76992896"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -615,7 +632,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110290816"/>
+        <c:crossAx val="76994432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -623,7 +640,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="110290816"/>
+        <c:axId val="76994432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="42300"/>
@@ -649,7 +666,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="110289280"/>
+        <c:crossAx val="76992896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="7"/>
@@ -703,13 +720,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>30693</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>635000</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>179917</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -727,6 +744,50 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>371475</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="114300" y="76200"/>
+          <a:ext cx="838200" cy="295275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1019,16 +1080,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AL11"/>
+  <dimension ref="A1:AL12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A38" sqref="A38"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" style="23" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" style="23" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" style="19" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" style="9" customWidth="1"/>
@@ -1050,140 +1111,143 @@
     <col min="37" max="38" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" s="4" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:38" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="24"/>
+      <c r="B1" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1"/>
+      <c r="M1"/>
+      <c r="N1"/>
+      <c r="O1"/>
+      <c r="P1"/>
+      <c r="Q1"/>
+      <c r="R1"/>
+      <c r="S1"/>
+      <c r="T1"/>
+      <c r="U1"/>
+      <c r="V1"/>
+      <c r="W1"/>
+      <c r="X1"/>
+      <c r="Y1"/>
+      <c r="Z1"/>
+      <c r="AA1"/>
+      <c r="AB1"/>
+      <c r="AC1"/>
+      <c r="AD1"/>
+      <c r="AE1"/>
+      <c r="AF1"/>
+      <c r="AG1"/>
+      <c r="AH1"/>
+      <c r="AI1"/>
+      <c r="AJ1"/>
+      <c r="AK1"/>
+      <c r="AL1"/>
+    </row>
+    <row r="2" spans="1:38" s="4" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H2" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I2" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="J2" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="K2" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
-      <c r="X1" s="6"/>
-      <c r="Y1" s="6"/>
-      <c r="Z1" s="6"/>
-      <c r="AA1" s="6"/>
-      <c r="AB1" s="6"/>
-      <c r="AC1" s="6"/>
-      <c r="AD1" s="6"/>
-      <c r="AE1" s="6"/>
-      <c r="AF1" s="6"/>
-      <c r="AG1" s="6"/>
-      <c r="AH1" s="6"/>
-      <c r="AI1" s="6"/>
-      <c r="AJ1" s="6"/>
-      <c r="AK1" s="7"/>
-      <c r="AL1" s="7"/>
-    </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="19">
-        <v>41989</v>
-      </c>
-      <c r="D2" s="9">
-        <v>6</v>
-      </c>
-      <c r="E2" s="9">
-        <v>5</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="13">
-        <f t="shared" ref="G2:G11" si="0">D2*7</f>
-        <v>42</v>
-      </c>
-      <c r="H2" s="21">
-        <f t="shared" ref="H2:H11" si="1">C2+(D2*7)</f>
-        <v>42031</v>
-      </c>
-      <c r="I2" s="16">
-        <f t="shared" ref="I2:I11" ca="1" si="2" xml:space="preserve"> IF( AND((TODAY() &gt; C2),(TODAY() &lt; H2)), TODAY()-C2, IF(TODAY()&lt;C2,0,G2))</f>
-        <v>42</v>
-      </c>
-      <c r="J2" s="16">
-        <f t="shared" ref="J2:J11" ca="1" si="3">IF(TODAY()&gt;H2, 0, G2-I2)</f>
-        <v>0</v>
-      </c>
-      <c r="K2" s="22" t="s">
-        <v>14</v>
-      </c>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
+      <c r="W2" s="6"/>
+      <c r="X2" s="6"/>
+      <c r="Y2" s="6"/>
+      <c r="Z2" s="6"/>
+      <c r="AA2" s="6"/>
+      <c r="AB2" s="6"/>
+      <c r="AC2" s="6"/>
+      <c r="AD2" s="6"/>
+      <c r="AE2" s="6"/>
+      <c r="AF2" s="6"/>
+      <c r="AG2" s="6"/>
+      <c r="AH2" s="6"/>
+      <c r="AI2" s="6"/>
+      <c r="AJ2" s="6"/>
+      <c r="AK2" s="7"/>
+      <c r="AL2" s="7"/>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
-        <v>28</v>
+      <c r="A3" s="22" t="s">
+        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C3" s="19">
-        <v>42009</v>
+        <v>41989</v>
       </c>
       <c r="D3" s="9">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E3" s="9">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G3" s="13">
-        <f t="shared" si="0"/>
-        <v>28</v>
+        <f t="shared" ref="G3:G12" si="0">D3*7</f>
+        <v>42</v>
       </c>
       <c r="H3" s="21">
-        <f t="shared" si="1"/>
-        <v>42037</v>
+        <f t="shared" ref="H3:H12" si="1">C3+(D3*7)</f>
+        <v>42031</v>
       </c>
       <c r="I3" s="16">
-        <f t="shared" ca="1" si="2"/>
-        <v>28</v>
+        <f t="shared" ref="I3:I12" ca="1" si="2" xml:space="preserve"> IF( AND((TODAY() &gt; C3),(TODAY() &lt; H3)), TODAY()-C3, IF(TODAY()&lt;C3,0,G3))</f>
+        <v>42</v>
       </c>
       <c r="J3" s="16">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ref="J3:J12" ca="1" si="3">IF(TODAY()&gt;H3, 0, G3-I3)</f>
         <v>0</v>
       </c>
       <c r="K3" s="22" t="s">
@@ -1192,13 +1256,13 @@
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C4" s="19">
-        <v>42037</v>
+        <v>42009</v>
       </c>
       <c r="D4" s="9">
         <v>4</v>
@@ -1215,7 +1279,7 @@
       </c>
       <c r="H4" s="21">
         <f t="shared" si="1"/>
-        <v>42065</v>
+        <v>42037</v>
       </c>
       <c r="I4" s="16">
         <f t="shared" ca="1" si="2"/>
@@ -1230,35 +1294,35 @@
       </c>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="20">
-        <v>42030</v>
-      </c>
-      <c r="D5" s="11">
-        <v>8</v>
-      </c>
-      <c r="E5" s="11">
+      <c r="A5" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="19">
+        <v>42037</v>
+      </c>
+      <c r="D5" s="9">
         <v>4</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="E5" s="9">
+        <v>9</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G5" s="13">
         <f t="shared" si="0"/>
-        <v>56</v>
+        <v>28</v>
       </c>
       <c r="H5" s="21">
         <f t="shared" si="1"/>
-        <v>42086</v>
+        <v>42065</v>
       </c>
       <c r="I5" s="16">
         <f t="shared" ca="1" si="2"/>
-        <v>56</v>
+        <v>28</v>
       </c>
       <c r="J5" s="16">
         <f t="shared" ca="1" si="3"/>
@@ -1269,120 +1333,120 @@
       </c>
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="19">
-        <v>42065</v>
-      </c>
-      <c r="D6" s="9">
+      <c r="A6" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="20">
+        <v>42030</v>
+      </c>
+      <c r="D6" s="11">
+        <v>8</v>
+      </c>
+      <c r="E6" s="11">
         <v>4</v>
       </c>
-      <c r="E6" s="9">
-        <v>9</v>
-      </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G6" s="13">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="H6" s="21">
         <f t="shared" si="1"/>
-        <v>42093</v>
+        <v>42086</v>
       </c>
       <c r="I6" s="16">
         <f t="shared" ca="1" si="2"/>
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="J6" s="16">
         <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="K6" s="22" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="18">
-        <v>42093</v>
-      </c>
-      <c r="D7" s="5">
-        <v>8</v>
-      </c>
-      <c r="E7" s="5">
-        <v>5</v>
+      <c r="A7" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="19">
+        <v>42065</v>
+      </c>
+      <c r="D7" s="9">
+        <v>4</v>
+      </c>
+      <c r="E7" s="9">
+        <v>9</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
-        <v>56</v>
+        <v>28</v>
       </c>
       <c r="H7" s="21">
         <f t="shared" si="1"/>
-        <v>42149</v>
+        <v>42093</v>
       </c>
       <c r="I7" s="16">
         <f t="shared" ca="1" si="2"/>
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="J7" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="K7" s="22" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A8" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="19">
+      <c r="A8" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="18">
         <v>42093</v>
       </c>
-      <c r="D8" s="9">
-        <v>4</v>
-      </c>
-      <c r="E8" s="9">
-        <v>9</v>
+      <c r="D8" s="5">
+        <v>8</v>
+      </c>
+      <c r="E8" s="5">
+        <v>5</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="H8" s="21">
         <f t="shared" si="1"/>
-        <v>42121</v>
+        <v>42149</v>
       </c>
       <c r="I8" s="16">
         <f t="shared" ca="1" si="2"/>
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="J8" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="K8" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.25">
@@ -1390,10 +1454,10 @@
         <v>16</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="19">
-        <v>42124</v>
+        <v>42093</v>
       </c>
       <c r="D9" s="9">
         <v>4</v>
@@ -1410,15 +1474,15 @@
       </c>
       <c r="H9" s="21">
         <f t="shared" si="1"/>
-        <v>42152</v>
+        <v>42121</v>
       </c>
       <c r="I9" s="16">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="J9" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="K9" s="22" t="s">
         <v>13</v>
@@ -1426,13 +1490,13 @@
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" s="19">
-        <v>42156</v>
+        <v>42124</v>
       </c>
       <c r="D10" s="9">
         <v>4</v>
@@ -1449,7 +1513,7 @@
       </c>
       <c r="H10" s="21">
         <f t="shared" si="1"/>
-        <v>42184</v>
+        <v>42152</v>
       </c>
       <c r="I10" s="16">
         <f t="shared" ca="1" si="2"/>
@@ -1464,28 +1528,31 @@
       </c>
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A11" s="23" t="s">
+        <v>28</v>
+      </c>
       <c r="B11" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" s="19">
         <v>42156</v>
       </c>
       <c r="D11" s="9">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E11" s="9">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
-        <v>70</v>
+        <v>28</v>
       </c>
       <c r="H11" s="21">
         <f t="shared" si="1"/>
-        <v>42226</v>
+        <v>42184</v>
       </c>
       <c r="I11" s="16">
         <f t="shared" ca="1" si="2"/>
@@ -1493,14 +1560,50 @@
       </c>
       <c r="J11" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>70</v>
+        <v>28</v>
       </c>
       <c r="K11" s="22" t="s">
         <v>13</v>
       </c>
     </row>
+    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="19">
+        <v>42156</v>
+      </c>
+      <c r="D12" s="9">
+        <v>10</v>
+      </c>
+      <c r="E12" s="9">
+        <v>8</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="13">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="H12" s="21">
+        <f t="shared" si="1"/>
+        <v>42226</v>
+      </c>
+      <c r="I12" s="16">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J12" s="16">
+        <f t="shared" ca="1" si="3"/>
+        <v>70</v>
+      </c>
+      <c r="K12" s="22" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:K11">
+  <autoFilter ref="A2:K12">
     <sortState ref="A2:K14">
       <sortCondition ref="H1:H14"/>
     </sortState>

</xml_diff>

<commit_message>
Added reference to the file in the README
</commit_message>
<xml_diff>
--- a/Courses Schedule.xlsx
+++ b/Courses Schedule.xlsx
@@ -619,11 +619,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="76992896"/>
-        <c:axId val="76994432"/>
+        <c:axId val="89051520"/>
+        <c:axId val="89053056"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="76992896"/>
+        <c:axId val="89051520"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -632,7 +632,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76994432"/>
+        <c:crossAx val="89053056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -640,7 +640,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="76994432"/>
+        <c:axId val="89053056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="42300"/>
@@ -666,7 +666,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="76992896"/>
+        <c:crossAx val="89051520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="7"/>

</xml_diff>

<commit_message>
Updated the license notice
</commit_message>
<xml_diff>
--- a/Courses Schedule.xlsx
+++ b/Courses Schedule.xlsx
@@ -129,7 +129,7 @@
     <t>Specialization: Z</t>
   </si>
   <si>
-    <t>This work is licensed under a Creative Commons Attribution 4.0 International License.</t>
+    <t>Courses Timeline Sheet by Ahmad Al-Kashef is licensed under a Creative Commons Attribution 4.0 International License.</t>
   </si>
 </sst>
 </file>
@@ -498,10 +498,10 @@
                   <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>17</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -591,10 +591,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>39</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>28</c:v>
@@ -619,11 +619,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="89051520"/>
-        <c:axId val="89053056"/>
+        <c:axId val="44438656"/>
+        <c:axId val="44440192"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="89051520"/>
+        <c:axId val="44438656"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -632,7 +632,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89053056"/>
+        <c:crossAx val="44440192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -640,7 +640,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="89053056"/>
+        <c:axId val="44440192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="42300"/>
@@ -666,7 +666,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="89051520"/>
+        <c:crossAx val="44438656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="7"/>
@@ -1084,7 +1084,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1439,11 +1439,11 @@
       </c>
       <c r="I8" s="16">
         <f t="shared" ca="1" si="2"/>
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="J8" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="K8" s="22" t="s">
         <v>12</v>
@@ -1478,11 +1478,11 @@
       </c>
       <c r="I9" s="16">
         <f t="shared" ca="1" si="2"/>
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="J9" s="16">
         <f t="shared" ca="1" si="3"/>
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="K9" s="22" t="s">
         <v>13</v>

</xml_diff>